<commit_message>
Correct named range for lever descriptions in mockay_calculator.xlsx
</commit_message>
<xml_diff>
--- a/tests/test_model/mockay_calculator.xlsx
+++ b/tests/test_model/mockay_calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccaveayl\vmware_shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3D7EB6-D6EF-4923-9A6F-B6A0A46B05DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D7E2A9-AC54-4985-AD78-6D35A838AF7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="OUTPUT.a">Model!$A$2:$S$2</definedName>
     <definedName name="OUTPUT.B">Model!$A$3:$S$3</definedName>
     <definedName name="output.land.map.area">Model!$A$4:$S$6</definedName>
-    <definedName name="output.lever.descriptions">Control!$F$2:$K$3</definedName>
+    <definedName name="output.lever.descriptions">Control!$G$2:$K$3</definedName>
     <definedName name="output.lever.example.ambition">Control!$F$1:$F$3</definedName>
     <definedName name="output.lever.group1">Control!$A$2:$B$2</definedName>
     <definedName name="output.lever.group2">Control!$A$3:$B$3</definedName>
@@ -669,16 +669,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B1" s="5">
         <v>2015</v>
       </c>
@@ -734,7 +734,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>35</v>
       </c>
@@ -811,7 +811,7 @@
         <v>2071</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>36</v>
       </c>
@@ -888,7 +888,7 @@
         <v>2061</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
@@ -897,7 +897,7 @@
         <v>40300</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:S6" si="0">20*C$1</f>
+        <f t="shared" ref="C4:S4" si="0">20*C$1</f>
         <v>40400</v>
       </c>
       <c r="D4">
@@ -965,7 +965,7 @@
         <v>42000</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>44100</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>34</v>
       </c>
@@ -1129,20 +1129,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1261,17 +1261,17 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="43.5703125" customWidth="1"/>
-    <col min="7" max="7" width="33.42578125" customWidth="1"/>
+    <col min="6" max="6" width="43.5546875" customWidth="1"/>
+    <col min="7" max="7" width="33.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1386,8 +1386,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D10" s="1" t="s">
         <v>59</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="3" t="s">
         <v>60</v>
       </c>

</xml_diff>